<commit_message>
Top 100 coins and Ether. classic
</commit_message>
<xml_diff>
--- a/files/coinmarketcap-july-21-8am.xlsx
+++ b/files/coinmarketcap-july-21-8am.xlsx
@@ -8,23 +8,31 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ak\xfer\proposals\mdc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{5B90B638-1E87-4F72-9295-1AE6392E5F2D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{3034294D-CF89-4AB1-9F70-7CBA59F8EF6B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Top100Coins" sheetId="1" r:id="rId1"/>
+    <sheet name="Ether_classic" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Top100Coins!$A$1:$H$101</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
   <fileRecoveryPr repairLoad="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="238">
   <si>
     <t>BTC</t>
   </si>
@@ -627,6 +635,117 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Jul 20, 2019</t>
+  </si>
+  <si>
+    <t>Jul 19, 2019</t>
+  </si>
+  <si>
+    <t>Jul 18, 2019</t>
+  </si>
+  <si>
+    <t>Jul 17, 2019</t>
+  </si>
+  <si>
+    <t>Jul 16, 2019</t>
+  </si>
+  <si>
+    <t>Jul 15, 2019</t>
+  </si>
+  <si>
+    <t>Jul 14, 2019</t>
+  </si>
+  <si>
+    <t>Jul 13, 2019</t>
+  </si>
+  <si>
+    <t>Jul 12, 2019</t>
+  </si>
+  <si>
+    <t>Jul 11, 2019</t>
+  </si>
+  <si>
+    <t>Jul 10, 2019</t>
+  </si>
+  <si>
+    <t>Jul 09, 2019</t>
+  </si>
+  <si>
+    <t>Jul 08, 2019</t>
+  </si>
+  <si>
+    <t>Jul 07, 2019</t>
+  </si>
+  <si>
+    <t>Jul 06, 2019</t>
+  </si>
+  <si>
+    <t>Jul 05, 2019</t>
+  </si>
+  <si>
+    <t>Jul 04, 2019</t>
+  </si>
+  <si>
+    <t>Jul 03, 2019</t>
+  </si>
+  <si>
+    <t>Jul 02, 2019</t>
+  </si>
+  <si>
+    <t>Jul 01, 2019</t>
+  </si>
+  <si>
+    <t>Jun 30, 2019</t>
+  </si>
+  <si>
+    <t>Jun 29, 2019</t>
+  </si>
+  <si>
+    <t>Jun 28, 2019</t>
+  </si>
+  <si>
+    <t>Jun 27, 2019</t>
+  </si>
+  <si>
+    <t>Jun 26, 2019</t>
+  </si>
+  <si>
+    <t>Jun 25, 2019</t>
+  </si>
+  <si>
+    <t>Jun 24, 2019</t>
+  </si>
+  <si>
+    <t>Jun 23, 2019</t>
+  </si>
+  <si>
+    <t>Jun 22, 2019</t>
+  </si>
+  <si>
+    <t>Jun 21, 2019</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Close</t>
+  </si>
+  <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t>ChangePct</t>
   </si>
 </sst>
 </file>
@@ -674,13 +793,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -696,6 +816,1014 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Ether_classic!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ChangePct</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Ether_classic!$A$2:$A$31</c:f>
+              <c:strCache>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>Jul 20, 2019</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Jul 19, 2019</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Jul 18, 2019</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Jul 17, 2019</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Jul 16, 2019</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Jul 15, 2019</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jul 14, 2019</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Jul 13, 2019</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Jul 12, 2019</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Jul 11, 2019</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Jul 10, 2019</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Jul 09, 2019</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Jul 08, 2019</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Jul 07, 2019</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Jul 06, 2019</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Jul 05, 2019</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Jul 04, 2019</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Jul 03, 2019</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Jul 02, 2019</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Jul 01, 2019</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Jun 30, 2019</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Jun 29, 2019</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Jun 28, 2019</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Jun 27, 2019</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Jun 26, 2019</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Jun 25, 2019</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Jun 24, 2019</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Jun 23, 2019</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Jun 22, 2019</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>Jun 21, 2019</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Ether_classic!$H$2:$H$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>5.2810902896081702</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-3.1353135313531273</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.1403508771929758</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.741573033707871</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-7.599309153713306</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.9366197183098648</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-14.608433734939755</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-2.643171806167397</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.5602409638554207</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-9.1780821917808222</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-7.7215189873417751</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-1.371571072319195</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.62735257214554363</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.5364916773367492</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-0.382653061224493</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.1612903225806432</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-1.020408163265307</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.0752269779507153</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-0.77319587628865483</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.64850843060959562</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-6.5296251511487204</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.9887920298879234</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.6936114732724832</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-15.188470066518839</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-2.2702702702702795</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-0.21574973031283251</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-0.21551724137930578</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.5317286652078641</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.6964490263459346</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.5882352941176547</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B414-4424-9BB0-F2E60D593184}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="606213144"/>
+        <c:axId val="606205600"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="606213144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="606205600"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="606205600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="606213144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>214312</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>157161</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{084CDB0E-2285-4039-9221-2DEFD441ACFB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1022,9 +2150,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A102" sqref="A102"/>
+      <selection pane="bottomLeft" activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3669,4 +4797,864 @@
   <autoFilter ref="A1:H101" xr:uid="{223B5070-AA57-403D-944A-D9E28E915711}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{124B1B44-ED27-441B-B23E-58408979B663}">
+  <dimension ref="A1:H31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N34" sqref="N34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="B2">
+        <v>5.87</v>
+      </c>
+      <c r="C2">
+        <v>6.32</v>
+      </c>
+      <c r="D2">
+        <v>5.86</v>
+      </c>
+      <c r="E2">
+        <v>6.18</v>
+      </c>
+      <c r="F2" s="1">
+        <v>550207510</v>
+      </c>
+      <c r="G2" s="1">
+        <v>692456633</v>
+      </c>
+      <c r="H2">
+        <f>100*(E2-B2)/B2</f>
+        <v>5.2810902896081702</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="B3">
+        <v>6.06</v>
+      </c>
+      <c r="C3">
+        <v>6.06</v>
+      </c>
+      <c r="D3">
+        <v>5.71</v>
+      </c>
+      <c r="E3">
+        <v>5.87</v>
+      </c>
+      <c r="F3" s="1">
+        <v>575039548</v>
+      </c>
+      <c r="G3" s="1">
+        <v>658174271</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H31" si="0">100*(E3-B3)/B3</f>
+        <v>-3.1353135313531273</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="B4">
+        <v>5.7</v>
+      </c>
+      <c r="C4">
+        <v>6.09</v>
+      </c>
+      <c r="D4">
+        <v>5.46</v>
+      </c>
+      <c r="E4">
+        <v>6.05</v>
+      </c>
+      <c r="F4" s="1">
+        <v>615658793</v>
+      </c>
+      <c r="G4" s="1">
+        <v>678427377</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>6.1403508771929758</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="B5">
+        <v>5.34</v>
+      </c>
+      <c r="C5">
+        <v>5.89</v>
+      </c>
+      <c r="D5">
+        <v>5.25</v>
+      </c>
+      <c r="E5">
+        <v>5.7</v>
+      </c>
+      <c r="F5" s="1">
+        <v>620406765</v>
+      </c>
+      <c r="G5" s="1">
+        <v>638731584</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>6.741573033707871</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="B6">
+        <v>5.79</v>
+      </c>
+      <c r="C6">
+        <v>6.07</v>
+      </c>
+      <c r="D6">
+        <v>5.22</v>
+      </c>
+      <c r="E6">
+        <v>5.35</v>
+      </c>
+      <c r="F6" s="1">
+        <v>659446809</v>
+      </c>
+      <c r="G6" s="1">
+        <v>598862271</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>-7.599309153713306</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="B7">
+        <v>5.68</v>
+      </c>
+      <c r="C7">
+        <v>5.85</v>
+      </c>
+      <c r="D7">
+        <v>5.22</v>
+      </c>
+      <c r="E7">
+        <v>5.79</v>
+      </c>
+      <c r="F7" s="1">
+        <v>684348176</v>
+      </c>
+      <c r="G7" s="1">
+        <v>648349211</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>1.9366197183098648</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B8">
+        <v>6.64</v>
+      </c>
+      <c r="C8">
+        <v>6.66</v>
+      </c>
+      <c r="D8">
+        <v>5.66</v>
+      </c>
+      <c r="E8">
+        <v>5.67</v>
+      </c>
+      <c r="F8" s="1">
+        <v>635115700</v>
+      </c>
+      <c r="G8" s="1">
+        <v>634811915</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>-14.608433734939755</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="B9">
+        <v>6.81</v>
+      </c>
+      <c r="C9">
+        <v>6.82</v>
+      </c>
+      <c r="D9">
+        <v>6.45</v>
+      </c>
+      <c r="E9">
+        <v>6.63</v>
+      </c>
+      <c r="F9" s="1">
+        <v>494753959</v>
+      </c>
+      <c r="G9" s="1">
+        <v>741892587</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>-2.643171806167397</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="B10">
+        <v>6.64</v>
+      </c>
+      <c r="C10">
+        <v>6.86</v>
+      </c>
+      <c r="D10">
+        <v>6.56</v>
+      </c>
+      <c r="E10">
+        <v>6.81</v>
+      </c>
+      <c r="F10" s="1">
+        <v>578739666</v>
+      </c>
+      <c r="G10" s="1">
+        <v>761680524</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>2.5602409638554207</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="B11">
+        <v>7.3</v>
+      </c>
+      <c r="C11">
+        <v>7.3</v>
+      </c>
+      <c r="D11">
+        <v>6.33</v>
+      </c>
+      <c r="E11">
+        <v>6.63</v>
+      </c>
+      <c r="F11" s="1">
+        <v>671496898</v>
+      </c>
+      <c r="G11" s="1">
+        <v>742236266</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>-9.1780821917808222</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="B12">
+        <v>7.9</v>
+      </c>
+      <c r="C12">
+        <v>7.94</v>
+      </c>
+      <c r="D12">
+        <v>7.02</v>
+      </c>
+      <c r="E12">
+        <v>7.29</v>
+      </c>
+      <c r="F12" s="1">
+        <v>674630757</v>
+      </c>
+      <c r="G12" s="1">
+        <v>815753606</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>-7.7215189873417751</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="B13">
+        <v>8.02</v>
+      </c>
+      <c r="C13">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="D13">
+        <v>7.81</v>
+      </c>
+      <c r="E13">
+        <v>7.91</v>
+      </c>
+      <c r="F13" s="1">
+        <v>654848641</v>
+      </c>
+      <c r="G13" s="1">
+        <v>884059262</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>-1.371571072319195</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="B14">
+        <v>7.97</v>
+      </c>
+      <c r="C14">
+        <v>8.0299999999999994</v>
+      </c>
+      <c r="D14">
+        <v>7.88</v>
+      </c>
+      <c r="E14">
+        <v>8.02</v>
+      </c>
+      <c r="F14" s="1">
+        <v>684112433</v>
+      </c>
+      <c r="G14" s="1">
+        <v>896184239</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>0.62735257214554363</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="B15">
+        <v>7.81</v>
+      </c>
+      <c r="C15">
+        <v>8.01</v>
+      </c>
+      <c r="D15">
+        <v>7.74</v>
+      </c>
+      <c r="E15">
+        <v>7.93</v>
+      </c>
+      <c r="F15" s="1">
+        <v>666411772</v>
+      </c>
+      <c r="G15" s="1">
+        <v>886493089</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>1.5364916773367492</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="B16">
+        <v>7.84</v>
+      </c>
+      <c r="C16">
+        <v>7.97</v>
+      </c>
+      <c r="D16">
+        <v>7.74</v>
+      </c>
+      <c r="E16">
+        <v>7.81</v>
+      </c>
+      <c r="F16" s="1">
+        <v>707657234</v>
+      </c>
+      <c r="G16" s="1">
+        <v>873272981</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>-0.382653061224493</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="B17">
+        <v>7.75</v>
+      </c>
+      <c r="C17">
+        <v>7.92</v>
+      </c>
+      <c r="D17">
+        <v>7.62</v>
+      </c>
+      <c r="E17">
+        <v>7.84</v>
+      </c>
+      <c r="F17" s="1">
+        <v>750356955</v>
+      </c>
+      <c r="G17" s="1">
+        <v>876290239</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>1.1612903225806432</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="B18">
+        <v>7.84</v>
+      </c>
+      <c r="C18">
+        <v>8.15</v>
+      </c>
+      <c r="D18">
+        <v>7.72</v>
+      </c>
+      <c r="E18">
+        <v>7.76</v>
+      </c>
+      <c r="F18" s="1">
+        <v>822719239</v>
+      </c>
+      <c r="G18" s="1">
+        <v>866756149</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>-1.020408163265307</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="B19">
+        <v>7.71</v>
+      </c>
+      <c r="C19">
+        <v>7.91</v>
+      </c>
+      <c r="D19">
+        <v>7.65</v>
+      </c>
+      <c r="E19">
+        <v>7.87</v>
+      </c>
+      <c r="F19" s="1">
+        <v>789429913</v>
+      </c>
+      <c r="G19" s="1">
+        <v>879061113</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>2.0752269779507153</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="B20">
+        <v>7.76</v>
+      </c>
+      <c r="C20">
+        <v>7.86</v>
+      </c>
+      <c r="D20">
+        <v>7.32</v>
+      </c>
+      <c r="E20">
+        <v>7.7</v>
+      </c>
+      <c r="F20" s="1">
+        <v>855230260</v>
+      </c>
+      <c r="G20" s="1">
+        <v>860313611</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>-0.77319587628865483</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="B21">
+        <v>7.71</v>
+      </c>
+      <c r="C21">
+        <v>7.98</v>
+      </c>
+      <c r="D21">
+        <v>7.33</v>
+      </c>
+      <c r="E21">
+        <v>7.76</v>
+      </c>
+      <c r="F21" s="1">
+        <v>874437054</v>
+      </c>
+      <c r="G21" s="1">
+        <v>866687455</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>0.64850843060959562</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="B22">
+        <v>8.27</v>
+      </c>
+      <c r="C22">
+        <v>8.6199999999999992</v>
+      </c>
+      <c r="D22">
+        <v>7.73</v>
+      </c>
+      <c r="E22">
+        <v>7.73</v>
+      </c>
+      <c r="F22" s="1">
+        <v>892040483</v>
+      </c>
+      <c r="G22" s="1">
+        <v>862249987</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="0"/>
+        <v>-6.5296251511487204</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="B23">
+        <v>8.0299999999999994</v>
+      </c>
+      <c r="C23">
+        <v>8.2899999999999991</v>
+      </c>
+      <c r="D23">
+        <v>7.62</v>
+      </c>
+      <c r="E23">
+        <v>8.27</v>
+      </c>
+      <c r="F23" s="1">
+        <v>810346203</v>
+      </c>
+      <c r="G23" s="1">
+        <v>923240201</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="0"/>
+        <v>2.9887920298879234</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="B24">
+        <v>7.67</v>
+      </c>
+      <c r="C24">
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="D24">
+        <v>7.55</v>
+      </c>
+      <c r="E24">
+        <v>8.0299999999999994</v>
+      </c>
+      <c r="F24" s="1">
+        <v>975712142</v>
+      </c>
+      <c r="G24" s="1">
+        <v>895508296</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="0"/>
+        <v>4.6936114732724832</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="B25">
+        <v>9.02</v>
+      </c>
+      <c r="C25">
+        <v>9.11</v>
+      </c>
+      <c r="D25">
+        <v>7.18</v>
+      </c>
+      <c r="E25">
+        <v>7.65</v>
+      </c>
+      <c r="F25" s="1">
+        <v>1407240749</v>
+      </c>
+      <c r="G25" s="1">
+        <v>853564080</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="0"/>
+        <v>-15.188470066518839</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="B26">
+        <v>9.25</v>
+      </c>
+      <c r="C26">
+        <v>9.6199999999999992</v>
+      </c>
+      <c r="D26">
+        <v>8.85</v>
+      </c>
+      <c r="E26">
+        <v>9.0399999999999991</v>
+      </c>
+      <c r="F26" s="1">
+        <v>1216912857</v>
+      </c>
+      <c r="G26" s="1">
+        <v>1008099057</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="0"/>
+        <v>-2.2702702702702795</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="B27">
+        <v>9.27</v>
+      </c>
+      <c r="C27">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D27">
+        <v>9.0500000000000007</v>
+      </c>
+      <c r="E27">
+        <v>9.25</v>
+      </c>
+      <c r="F27" s="1">
+        <v>769322239</v>
+      </c>
+      <c r="G27" s="1">
+        <v>1031488658</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="0"/>
+        <v>-0.21574973031283251</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="B28">
+        <v>9.2799999999999994</v>
+      </c>
+      <c r="C28">
+        <v>9.39</v>
+      </c>
+      <c r="D28">
+        <v>8.9700000000000006</v>
+      </c>
+      <c r="E28">
+        <v>9.26</v>
+      </c>
+      <c r="F28" s="1">
+        <v>771250120</v>
+      </c>
+      <c r="G28" s="1">
+        <v>1032361311</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="0"/>
+        <v>-0.21551724137930578</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="B29">
+        <v>9.14</v>
+      </c>
+      <c r="C29">
+        <v>9.59</v>
+      </c>
+      <c r="D29">
+        <v>9.06</v>
+      </c>
+      <c r="E29">
+        <v>9.2799999999999994</v>
+      </c>
+      <c r="F29" s="1">
+        <v>958883927</v>
+      </c>
+      <c r="G29" s="1">
+        <v>1033684279</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="0"/>
+        <v>1.5317286652078641</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="B30">
+        <v>8.73</v>
+      </c>
+      <c r="C30">
+        <v>9.2899999999999991</v>
+      </c>
+      <c r="D30">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="E30">
+        <v>9.14</v>
+      </c>
+      <c r="F30" s="1">
+        <v>1107874156</v>
+      </c>
+      <c r="G30" s="1">
+        <v>1018811434</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="0"/>
+        <v>4.6964490263459346</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="B31">
+        <v>8.5</v>
+      </c>
+      <c r="C31">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="D31">
+        <v>8.4499999999999993</v>
+      </c>
+      <c r="E31">
+        <v>8.7200000000000006</v>
+      </c>
+      <c r="F31" s="1">
+        <v>815961669</v>
+      </c>
+      <c r="G31" s="1">
+        <v>971357363</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="0"/>
+        <v>2.5882352941176547</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>